<commit_message>
finished all grammar checks using Grammarly Premium
</commit_message>
<xml_diff>
--- a/latex/images/growth-of-bureaucracy-plot.xlsx
+++ b/latex/images/growth-of-bureaucracy-plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlin/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D83D5DA-DA1A-994E-B60B-BE61F5539F86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA29B26D-24CF-A04C-9772-45340391C891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{5200DB4A-0644-3D4B-8A78-1930E594FC1D}"/>
   </bookViews>
@@ -136,8 +136,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12262489063867017"/>
-          <c:y val="5.5555555555555552E-2"/>
+          <c:x val="4.7624890638670161E-2"/>
+          <c:y val="2.7777777777777776E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -173,28 +173,28 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>branching=3</c:v>
+            <c:v>branching=7</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="triangle"/>
             <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="7030A0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -202,7 +202,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$16:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -229,7 +229,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>Sheet1!$D$16:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -237,19 +237,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69230769230769229</c:v>
+                  <c:v>0.85964912280701755</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67500000000000004</c:v>
+                  <c:v>0.85750000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66942148760330578</c:v>
+                  <c:v>0.85719385933595149</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66758241758241754</c:v>
+                  <c:v>0.85715014279885759</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -257,7 +257,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-235D-DE4F-BC00-648D1C8658BC}"/>
+              <c16:uniqueId val="{00000002-235D-DE4F-BC00-648D1C8658BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -351,28 +351,28 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>branching=7</c:v>
+            <c:v>branching=3</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="square"/>
             <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="7030A0"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -380,7 +380,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$21</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -407,7 +407,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$21</c:f>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -415,19 +415,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.875</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85964912280701755</c:v>
+                  <c:v>0.69230769230769229</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.85750000000000004</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.85719385933595149</c:v>
+                  <c:v>0.66942148760330578</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.85715014279885759</c:v>
+                  <c:v>0.66758241758241754</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,7 +435,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-235D-DE4F-BC00-648D1C8658BC}"/>
+              <c16:uniqueId val="{00000000-235D-DE4F-BC00-648D1C8658BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -454,11 +454,25 @@
         <c:axId val="2130005247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6.5"/>
+          <c:max val="6"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -674,6 +688,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7753462379702537"/>
+          <c:y val="0.37532261592300964"/>
+          <c:w val="0.2218759842519685"/>
+          <c:h val="0.28477143482064743"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1304,16 +1328,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>